<commit_message>
save dra survey feedback
</commit_message>
<xml_diff>
--- a/tests/User Test Feedback/test results summary.xlsx
+++ b/tests/User Test Feedback/test results summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sype\Downloads\Moodle4.0\server\moodle\blocks\gradeup\tests\User Test Feedback\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF51FCA-D9C1-4CC7-9862-0E5F98C575E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4BFB6F2-0D42-4442-9C60-1948915EF250}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>tyler</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>OK</t>
+  </si>
+  <si>
+    <t>dr A</t>
   </si>
 </sst>
 </file>
@@ -553,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +568,7 @@
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -581,8 +584,11 @@
       <c r="F1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
@@ -601,8 +607,11 @@
       <c r="F2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>6</v>
       </c>
@@ -621,8 +630,11 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>7</v>
       </c>
@@ -641,8 +653,11 @@
       <c r="F4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>8</v>
       </c>
@@ -661,8 +676,11 @@
       <c r="F5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
@@ -681,8 +699,11 @@
       <c r="F6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
@@ -701,8 +722,11 @@
       <c r="F7">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -721,8 +745,11 @@
       <c r="F8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -741,8 +768,11 @@
       <c r="F9">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>
@@ -761,8 +791,11 @@
       <c r="F10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
@@ -781,8 +814,11 @@
       <c r="F11">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -800,6 +836,9 @@
       </c>
       <c r="F12" t="s">
         <v>21</v>
+      </c>
+      <c r="G12" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>